<commit_message>
Modified fr databook loads
</commit_message>
<xml_diff>
--- a/nutrition/legacy_default_params.xlsx
+++ b/nutrition/legacy_default_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/nutrition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\nutrition\nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E48B666-71F4-E74A-9905-930C7C52D20A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5BFDF9-06E6-400F-A0B1-9649BEA1ACF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2775" yWindow="810" windowWidth="21660" windowHeight="19935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs impacted population" sheetId="14" r:id="rId1"/>
@@ -44,10 +44,19 @@
     <definedName name="stillbirth">'[1]Baseline year population inputs'!$C$27</definedName>
     <definedName name="term_SGA">'[1]Baseline year population inputs'!$C$35</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -660,8 +669,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -810,7 +819,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -879,7 +888,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1252,23 +1261,23 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="41" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="41" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.83203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.83203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.1640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.875" style="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.875" style="41" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.125" style="41" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="14.5" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>116</v>
       </c>
@@ -1315,7 +1324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>115</v>
       </c>
@@ -1362,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="54" t="s">
         <v>127</v>
       </c>
@@ -1406,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="54" t="s">
         <v>114</v>
       </c>
@@ -1450,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="54" t="s">
         <v>113</v>
       </c>
@@ -1494,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="54" t="s">
         <v>112</v>
       </c>
@@ -1538,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="54" t="s">
         <v>152</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="54" t="s">
         <v>61</v>
       </c>
@@ -1626,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="54" t="s">
         <v>79</v>
       </c>
@@ -1670,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="54" t="s">
         <v>87</v>
       </c>
@@ -1714,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="54" t="s">
         <v>62</v>
       </c>
@@ -1758,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="54" t="s">
         <v>82</v>
       </c>
@@ -1802,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="54" t="s">
         <v>96</v>
       </c>
@@ -1846,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="54" t="s">
         <v>86</v>
       </c>
@@ -1890,7 +1899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="54" t="s">
         <v>89</v>
       </c>
@@ -1934,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="54"/>
       <c r="C16" s="46"/>
       <c r="D16" s="46"/>
@@ -1950,7 +1959,7 @@
       <c r="N16" s="46"/>
       <c r="O16" s="46"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
         <v>106</v>
       </c>
@@ -1997,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43"/>
       <c r="B18" s="54" t="s">
         <v>101</v>
@@ -2042,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="34" t="s">
         <v>148</v>
       </c>
@@ -2086,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="34" t="s">
         <v>158</v>
       </c>
@@ -2130,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="55" t="s">
         <v>70</v>
       </c>
@@ -2174,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="54" t="s">
         <v>99</v>
       </c>
@@ -2218,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="54" t="s">
         <v>100</v>
       </c>
@@ -2262,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="54" t="s">
         <v>71</v>
       </c>
@@ -2306,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="54"/>
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
@@ -2322,7 +2331,7 @@
       <c r="N25" s="46"/>
       <c r="O25" s="46"/>
     </row>
-    <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
         <v>111</v>
       </c>
@@ -2370,7 +2379,7 @@
       </c>
       <c r="P26" s="56"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="35" t="s">
         <v>149</v>
       </c>
@@ -2414,7 +2423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="43"/>
       <c r="B28" s="35" t="s">
         <v>159</v>
@@ -2459,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="35" t="s">
         <v>150</v>
       </c>
@@ -2503,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="35" t="s">
         <v>151</v>
       </c>
@@ -2547,7 +2556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="54"/>
       <c r="C31" s="45"/>
       <c r="D31" s="45"/>
@@ -2563,7 +2572,7 @@
       <c r="N31" s="46"/>
       <c r="O31" s="46"/>
     </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
         <v>110</v>
       </c>
@@ -2610,7 +2619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="54" t="s">
         <v>74</v>
       </c>
@@ -2654,7 +2663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="54" t="s">
         <v>76</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="54" t="s">
         <v>77</v>
       </c>
@@ -2742,7 +2751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="54" t="s">
         <v>69</v>
       </c>
@@ -2786,7 +2795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="42"/>
       <c r="B37" s="54" t="s">
         <v>90</v>
@@ -2831,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="54" t="s">
         <v>91</v>
       </c>
@@ -2875,7 +2884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="54" t="s">
         <v>92</v>
       </c>
@@ -2919,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="54" t="s">
         <v>94</v>
       </c>
@@ -2963,7 +2972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="54" t="s">
         <v>93</v>
       </c>
@@ -3008,7 +3017,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B17:O24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B17:O24">
     <sortCondition ref="B17:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3026,15 +3035,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
     <col min="3" max="7" width="14" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="33"/>
       <c r="C1" s="2" t="s">
@@ -3053,12 +3062,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" s="35" t="s">
         <v>82</v>
       </c>
@@ -3078,7 +3087,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
@@ -3089,7 +3098,7 @@
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="34" t="s">
         <v>147</v>
       </c>
@@ -3126,20 +3135,20 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.6640625" style="54" customWidth="1"/>
+    <col min="1" max="1" width="47.625" style="54" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="54" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="54" customWidth="1"/>
+    <col min="3" max="3" width="22.375" style="54" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="1"/>
-    <col min="8" max="8" width="15.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.875" style="1" customWidth="1"/>
     <col min="9" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
@@ -3165,7 +3174,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
         <v>96</v>
       </c>
@@ -3191,7 +3200,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C3" s="54" t="s">
         <v>84</v>
       </c>
@@ -3211,7 +3220,7 @@
         <v>0.53134328358208949</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="54" t="s">
         <v>88</v>
       </c>
@@ -3231,7 +3240,7 @@
         <v>0.38507462686567184</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="54" t="s">
         <v>62</v>
       </c>
@@ -3257,7 +3266,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C6" s="54" t="s">
         <v>88</v>
       </c>
@@ -3277,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="54" t="s">
         <v>53</v>
       </c>
@@ -3300,7 +3309,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C8" s="54" t="s">
         <v>88</v>
       </c>
@@ -3320,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="54" t="s">
         <v>61</v>
       </c>
@@ -3346,7 +3355,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C10" s="54" t="s">
         <v>88</v>
       </c>
@@ -3366,7 +3375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="54" t="s">
         <v>53</v>
       </c>
@@ -3389,7 +3398,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C12" s="54" t="s">
         <v>88</v>
       </c>
@@ -3409,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="54" t="s">
         <v>95</v>
       </c>
@@ -3435,7 +3444,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" s="54" t="s">
         <v>88</v>
       </c>
@@ -3456,7 +3465,7 @@
       </c>
       <c r="I14" s="27"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="54" t="s">
         <v>53</v>
       </c>
@@ -3480,7 +3489,7 @@
       </c>
       <c r="I15" s="27"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16" s="54" t="s">
         <v>88</v>
       </c>
@@ -3501,7 +3510,7 @@
       </c>
       <c r="I16" s="27"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="54" t="s">
         <v>76</v>
       </c>
@@ -3528,7 +3537,7 @@
       </c>
       <c r="I17" s="27"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C18" s="54" t="s">
         <v>84</v>
       </c>
@@ -3549,7 +3558,7 @@
       </c>
       <c r="I18" s="27"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="54" t="s">
         <v>75</v>
       </c>
@@ -3575,7 +3584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C20" s="54" t="s">
         <v>84</v>
       </c>
@@ -3595,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
         <v>74</v>
       </c>
@@ -3621,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C22" s="54" t="s">
         <v>84</v>
       </c>
@@ -3641,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="54" t="s">
         <v>94</v>
       </c>
@@ -3667,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C24" s="54" t="s">
         <v>84</v>
       </c>
@@ -3687,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C25" s="54" t="s">
         <v>88</v>
       </c>
@@ -3707,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="54" t="s">
         <v>93</v>
       </c>
@@ -3733,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C27" s="54" t="s">
         <v>84</v>
       </c>
@@ -3753,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C28" s="54" t="s">
         <v>88</v>
       </c>
@@ -3773,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
         <v>92</v>
       </c>
@@ -3799,7 +3808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C30" s="54" t="s">
         <v>84</v>
       </c>
@@ -3819,7 +3828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C31" s="54" t="s">
         <v>88</v>
       </c>
@@ -3839,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="54" t="s">
         <v>91</v>
       </c>
@@ -3865,7 +3874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C33" s="54" t="s">
         <v>84</v>
       </c>
@@ -3885,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C34" s="54" t="s">
         <v>88</v>
       </c>
@@ -3905,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="54" t="s">
         <v>90</v>
       </c>
@@ -3931,7 +3940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C36" s="54" t="s">
         <v>84</v>
       </c>
@@ -3951,7 +3960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C37" s="54" t="s">
         <v>88</v>
       </c>
@@ -3971,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="54" t="s">
         <v>89</v>
       </c>
@@ -3997,7 +4006,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C39" s="54" t="s">
         <v>84</v>
       </c>
@@ -4017,7 +4026,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C40" s="54" t="s">
         <v>88</v>
       </c>
@@ -4037,7 +4046,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B41" s="54" t="s">
         <v>40</v>
       </c>
@@ -4060,7 +4069,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C42" s="54" t="s">
         <v>84</v>
       </c>
@@ -4080,7 +4089,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C43" s="54" t="s">
         <v>88</v>
       </c>
@@ -4100,7 +4109,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="54" t="s">
         <v>87</v>
       </c>
@@ -4126,7 +4135,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C45" s="54" t="s">
         <v>84</v>
       </c>
@@ -4146,7 +4155,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="54" t="s">
         <v>86</v>
       </c>
@@ -4172,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C47" s="54" t="s">
         <v>84</v>
       </c>
@@ -4192,7 +4201,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="54" t="s">
         <v>152</v>
       </c>
@@ -4218,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.15">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C49" s="54" t="s">
         <v>84</v>
       </c>
@@ -4255,16 +4264,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.375" style="1" customWidth="1"/>
     <col min="4" max="7" width="15.5" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>73</v>
       </c>
@@ -4286,7 +4295,7 @@
       </c>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>101</v>
       </c>
@@ -4310,7 +4319,7 @@
       </c>
       <c r="H2" s="34"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>84</v>
       </c>
@@ -4328,7 +4337,7 @@
       </c>
       <c r="H3" s="37"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>100</v>
       </c>
@@ -4352,7 +4361,7 @@
       </c>
       <c r="H4" s="37"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="C5" s="1" t="s">
         <v>84</v>
@@ -4371,7 +4380,7 @@
       </c>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>99</v>
       </c>
@@ -4395,7 +4404,7 @@
       </c>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="C7" s="1" t="s">
         <v>84</v>
@@ -4430,22 +4439,22 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
@@ -4480,7 +4489,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
         <v>72</v>
       </c>
@@ -4497,7 +4506,7 @@
       <c r="J2" s="50"/>
       <c r="K2" s="50"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="54" t="s">
         <v>101</v>
       </c>
@@ -4514,7 +4523,7 @@
       <c r="J3" s="50"/>
       <c r="K3" s="50"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="54" t="s">
         <v>95</v>
       </c>
@@ -4531,7 +4540,7 @@
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="54" t="s">
         <v>127</v>
       </c>
@@ -4548,7 +4557,7 @@
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="54" t="s">
         <v>118</v>
       </c>
@@ -4567,7 +4576,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="54" t="s">
         <v>75</v>
       </c>
@@ -4586,7 +4595,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
         <v>74</v>
       </c>
@@ -4605,7 +4614,7 @@
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="54" t="s">
         <v>76</v>
       </c>
@@ -4624,7 +4633,7 @@
       <c r="J9" s="50"/>
       <c r="K9" s="50"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
         <v>149</v>
       </c>
@@ -4641,7 +4650,7 @@
       <c r="J10" s="50"/>
       <c r="K10" s="50"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
         <v>159</v>
       </c>
@@ -4658,7 +4667,7 @@
       <c r="J11" s="50"/>
       <c r="K11" s="50"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
         <v>150</v>
       </c>
@@ -4675,7 +4684,7 @@
       <c r="J12" s="50"/>
       <c r="K12" s="50"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
         <v>151</v>
       </c>
@@ -4692,7 +4701,7 @@
       <c r="J13" s="50"/>
       <c r="K13" s="50"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
         <v>148</v>
       </c>
@@ -4711,7 +4720,7 @@
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="34" t="s">
         <v>158</v>
       </c>
@@ -4730,7 +4739,7 @@
       <c r="J15" s="50"/>
       <c r="K15" s="50"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="54" t="s">
         <v>70</v>
       </c>
@@ -4751,7 +4760,7 @@
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="54" t="s">
         <v>77</v>
       </c>
@@ -4768,7 +4777,7 @@
       <c r="J17" s="50"/>
       <c r="K17" s="50"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="54" t="s">
         <v>114</v>
       </c>
@@ -4787,7 +4796,7 @@
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="54" t="s">
         <v>113</v>
       </c>
@@ -4806,7 +4815,7 @@
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="54" t="s">
         <v>112</v>
       </c>
@@ -4825,7 +4834,7 @@
       <c r="J20" s="50"/>
       <c r="K20" s="50"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
         <v>152</v>
       </c>
@@ -4844,7 +4853,7 @@
       <c r="J21" s="50"/>
       <c r="K21" s="50"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="54" t="s">
         <v>61</v>
       </c>
@@ -4865,7 +4874,7 @@
       <c r="J22" s="50"/>
       <c r="K22" s="50"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="54" t="s">
         <v>69</v>
       </c>
@@ -4884,7 +4893,7 @@
       <c r="J23" s="50"/>
       <c r="K23" s="50"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="54" t="s">
         <v>99</v>
       </c>
@@ -4901,7 +4910,7 @@
       <c r="J24" s="50"/>
       <c r="K24" s="50"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="54" t="s">
         <v>100</v>
       </c>
@@ -4918,7 +4927,7 @@
       <c r="J25" s="50"/>
       <c r="K25" s="50"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="54" t="s">
         <v>79</v>
       </c>
@@ -4935,7 +4944,7 @@
       <c r="J26" s="50"/>
       <c r="K26" s="50"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="54" t="s">
         <v>71</v>
       </c>
@@ -4954,7 +4963,7 @@
       <c r="J27" s="50"/>
       <c r="K27" s="50"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="54" t="s">
         <v>87</v>
       </c>
@@ -4971,7 +4980,7 @@
       <c r="J28" s="50"/>
       <c r="K28" s="50"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
         <v>62</v>
       </c>
@@ -4990,7 +4999,7 @@
       <c r="J29" s="50"/>
       <c r="K29" s="50"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="54" t="s">
         <v>82</v>
       </c>
@@ -5007,7 +5016,7 @@
       <c r="J30" s="50"/>
       <c r="K30" s="50"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="54" t="s">
         <v>96</v>
       </c>
@@ -5026,7 +5035,7 @@
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="54" t="s">
         <v>90</v>
       </c>
@@ -5045,7 +5054,7 @@
       <c r="J32" s="50"/>
       <c r="K32" s="50"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="54" t="s">
         <v>91</v>
       </c>
@@ -5064,7 +5073,7 @@
       <c r="J33" s="50"/>
       <c r="K33" s="50"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="54" t="s">
         <v>92</v>
       </c>
@@ -5083,7 +5092,7 @@
       <c r="J34" s="50"/>
       <c r="K34" s="50"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="54" t="s">
         <v>94</v>
       </c>
@@ -5102,7 +5111,7 @@
       <c r="J35" s="50"/>
       <c r="K35" s="50"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="54" t="s">
         <v>93</v>
       </c>
@@ -5121,7 +5130,7 @@
       <c r="J36" s="50"/>
       <c r="K36" s="50"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="54" t="s">
         <v>86</v>
       </c>
@@ -5138,7 +5147,7 @@
       <c r="J37" s="50"/>
       <c r="K37" s="50"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="54" t="s">
         <v>89</v>
       </c>
@@ -5160,7 +5169,7 @@
       <c r="K38" s="50"/>
     </row>
   </sheetData>
-  <sortState ref="A2:J38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J38">
     <sortCondition ref="A2:A38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5178,22 +5187,22 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>126</v>
       </c>
@@ -5228,7 +5237,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -5257,7 +5266,7 @@
       <c r="J2" s="50"/>
       <c r="K2" s="50"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -5286,7 +5295,7 @@
       <c r="J3" s="50"/>
       <c r="K3" s="50"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -5315,7 +5324,7 @@
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -5344,7 +5353,7 @@
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -5373,7 +5382,7 @@
       <c r="J6" s="50"/>
       <c r="K6" s="50"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -5394,7 +5403,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -5415,7 +5424,7 @@
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -5436,7 +5445,7 @@
       <c r="J9" s="50"/>
       <c r="K9" s="50"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -5457,7 +5466,7 @@
       <c r="J10" s="50"/>
       <c r="K10" s="50"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -5478,7 +5487,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -5497,7 +5506,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -5516,7 +5525,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -5551,15 +5560,15 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>109</v>
       </c>
@@ -5585,7 +5594,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>133</v>
       </c>
@@ -5611,7 +5620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="57"/>
       <c r="C3" s="1" t="s">
         <v>104</v>
@@ -5633,7 +5642,7 @@
       </c>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="57"/>
       <c r="C4" s="1" t="s">
         <v>102</v>
@@ -5655,7 +5664,7 @@
       </c>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="57" t="s">
         <v>36</v>
       </c>
@@ -5679,7 +5688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="57"/>
       <c r="C6" s="1" t="s">
         <v>104</v>
@@ -5700,7 +5709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="57"/>
       <c r="C7" s="1" t="s">
         <v>102</v>
@@ -5721,7 +5730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="57" t="s">
         <v>35</v>
       </c>
@@ -5744,7 +5753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="57"/>
       <c r="C9" s="1" t="s">
         <v>104</v>
@@ -5765,7 +5774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="57"/>
       <c r="C10" s="1" t="s">
         <v>102</v>
@@ -5786,7 +5795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="57" t="s">
         <v>34</v>
       </c>
@@ -5809,7 +5818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="57"/>
       <c r="C12" s="1" t="s">
         <v>104</v>
@@ -5830,7 +5839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="57"/>
       <c r="C13" s="1" t="s">
         <v>102</v>
@@ -5851,7 +5860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="57" t="s">
         <v>33</v>
       </c>
@@ -5874,7 +5883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="57"/>
       <c r="C15" s="1" t="s">
         <v>104</v>
@@ -5895,7 +5904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="57"/>
       <c r="C16" s="1" t="s">
         <v>102</v>
@@ -5916,7 +5925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="38" t="s">
         <v>103</v>
       </c>
@@ -5939,7 +5948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>135</v>
       </c>
@@ -5965,7 +5974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B20" s="57"/>
       <c r="C20" s="1" t="s">
         <v>104</v>
@@ -5986,7 +5995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" s="57"/>
       <c r="C21" s="1" t="s">
         <v>102</v>
@@ -6007,7 +6016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" s="57" t="s">
         <v>36</v>
       </c>
@@ -6030,7 +6039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" s="57"/>
       <c r="C23" s="1" t="s">
         <v>104</v>
@@ -6051,7 +6060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24" s="57"/>
       <c r="C24" s="1" t="s">
         <v>102</v>
@@ -6072,7 +6081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B25" s="57" t="s">
         <v>35</v>
       </c>
@@ -6095,7 +6104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B26" s="57"/>
       <c r="C26" s="1" t="s">
         <v>104</v>
@@ -6116,7 +6125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B27" s="57"/>
       <c r="C27" s="1" t="s">
         <v>102</v>
@@ -6137,7 +6146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B28" s="57" t="s">
         <v>34</v>
       </c>
@@ -6160,7 +6169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B29" s="57"/>
       <c r="C29" s="1" t="s">
         <v>104</v>
@@ -6181,7 +6190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B30" s="57"/>
       <c r="C30" s="1" t="s">
         <v>102</v>
@@ -6202,7 +6211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B31" s="57" t="s">
         <v>33</v>
       </c>
@@ -6225,7 +6234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B32" s="57"/>
       <c r="C32" s="1" t="s">
         <v>104</v>
@@ -6246,7 +6255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B33" s="57"/>
       <c r="C33" s="1" t="s">
         <v>102</v>
@@ -6267,7 +6276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B34" s="38" t="s">
         <v>103</v>
       </c>
@@ -6290,7 +6299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="40" t="s">
         <v>134</v>
       </c>
@@ -6316,7 +6325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" s="57"/>
       <c r="C37" s="1" t="s">
         <v>104</v>
@@ -6337,7 +6346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B38" s="57"/>
       <c r="C38" s="1" t="s">
         <v>102</v>
@@ -6358,7 +6367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B39" s="57" t="s">
         <v>36</v>
       </c>
@@ -6381,7 +6390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B40" s="57"/>
       <c r="C40" s="1" t="s">
         <v>104</v>
@@ -6402,7 +6411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B41" s="57"/>
       <c r="C41" s="1" t="s">
         <v>102</v>
@@ -6423,7 +6432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" s="57" t="s">
         <v>35</v>
       </c>
@@ -6446,7 +6455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B43" s="57"/>
       <c r="C43" s="1" t="s">
         <v>104</v>
@@ -6467,7 +6476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B44" s="57"/>
       <c r="C44" s="1" t="s">
         <v>102</v>
@@ -6488,7 +6497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B45" s="57" t="s">
         <v>34</v>
       </c>
@@ -6511,7 +6520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" s="57"/>
       <c r="C46" s="1" t="s">
         <v>104</v>
@@ -6532,7 +6541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" s="57"/>
       <c r="C47" s="1" t="s">
         <v>102</v>
@@ -6553,7 +6562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B48" s="57" t="s">
         <v>33</v>
       </c>
@@ -6576,7 +6585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="57"/>
       <c r="C49" s="1" t="s">
         <v>104</v>
@@ -6597,7 +6606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="57"/>
       <c r="C50" s="1" t="s">
         <v>102</v>
@@ -6618,7 +6627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="39" t="s">
         <v>103</v>
       </c>
@@ -6643,6 +6652,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -6653,11 +6667,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6675,22 +6684,22 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="1" customWidth="1"/>
     <col min="5" max="6" width="13.5" style="1" customWidth="1"/>
     <col min="7" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="24"/>
       <c r="C2" s="23" t="s">
         <v>22</v>
@@ -6705,7 +6714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -6715,7 +6724,7 @@
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19" t="s">
         <v>18</v>
       </c>
@@ -6732,7 +6741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
         <v>17</v>
       </c>
@@ -6749,7 +6758,7 @@
         <v>3.03</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
@@ -6766,7 +6775,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
         <v>15</v>
       </c>
@@ -6783,13 +6792,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="13"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -6807,14 +6816,14 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="13"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
@@ -6824,7 +6833,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -6834,7 +6843,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -6852,7 +6861,7 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
@@ -6870,7 +6879,7 @@
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -6888,7 +6897,7 @@
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="12"/>
@@ -6897,7 +6906,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -6908,7 +6917,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
@@ -6926,7 +6935,7 @@
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
         <v>6</v>
       </c>
@@ -6944,7 +6953,7 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
@@ -6962,7 +6971,7 @@
       </c>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
@@ -6980,7 +6989,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
         <v>3</v>
       </c>
@@ -6997,7 +7006,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>2</v>
       </c>
@@ -7014,7 +7023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>1</v>
       </c>
@@ -7031,7 +7040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
         <v>0</v>
       </c>
@@ -7048,10 +7057,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
     </row>
   </sheetData>
@@ -7071,23 +7080,23 @@
       <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="1" customWidth="1"/>
-    <col min="4" max="8" width="13.33203125" style="1" customWidth="1"/>
-    <col min="9" max="12" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="13.375" style="1" customWidth="1"/>
+    <col min="9" max="12" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="15.125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>125</v>
       </c>
@@ -7121,7 +7130,7 @@
       <c r="O2" s="28"/>
       <c r="P2" s="28"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>41</v>
@@ -7153,7 +7162,7 @@
       <c r="O3" s="25"/>
       <c r="P3" s="25"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C4" s="26" t="s">
         <v>137</v>
       </c>
@@ -7181,7 +7190,7 @@
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C5" s="26" t="s">
         <v>138</v>
       </c>
@@ -7209,7 +7218,7 @@
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C6" s="26" t="s">
         <v>139</v>
       </c>
@@ -7237,7 +7246,7 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
@@ -7268,7 +7277,7 @@
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C8" s="26" t="s">
         <v>137</v>
       </c>
@@ -7296,7 +7305,7 @@
       <c r="O8" s="25"/>
       <c r="P8" s="25"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C9" s="26" t="s">
         <v>138</v>
       </c>
@@ -7324,7 +7333,7 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C10" s="26" t="s">
         <v>139</v>
       </c>
@@ -7352,7 +7361,7 @@
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
@@ -7383,7 +7392,7 @@
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C12" s="26" t="s">
         <v>137</v>
       </c>
@@ -7411,7 +7420,7 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C13" s="26" t="s">
         <v>138</v>
       </c>
@@ -7439,7 +7448,7 @@
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C14" s="26" t="s">
         <v>139</v>
       </c>
@@ -7467,7 +7476,7 @@
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
@@ -7498,7 +7507,7 @@
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C16" s="26" t="s">
         <v>137</v>
       </c>
@@ -7526,7 +7535,7 @@
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C17" s="26" t="s">
         <v>138</v>
       </c>
@@ -7554,7 +7563,7 @@
       <c r="O17" s="25"/>
       <c r="P17" s="25"/>
     </row>
-    <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="26" t="s">
         <v>139</v>
       </c>
@@ -7582,7 +7591,7 @@
       <c r="O18" s="25"/>
       <c r="P18" s="25"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B19" s="27" t="s">
         <v>39</v>
       </c>
@@ -7613,7 +7622,7 @@
       <c r="O19" s="25"/>
       <c r="P19" s="25"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C20" s="26" t="s">
         <v>137</v>
       </c>
@@ -7641,7 +7650,7 @@
       <c r="O20" s="25"/>
       <c r="P20" s="25"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C21" s="26" t="s">
         <v>138</v>
       </c>
@@ -7669,7 +7678,7 @@
       <c r="O21" s="25"/>
       <c r="P21" s="25"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C22" s="26" t="s">
         <v>139</v>
       </c>
@@ -7697,7 +7706,7 @@
       <c r="O22" s="25"/>
       <c r="P22" s="25"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B23" s="27" t="s">
         <v>47</v>
       </c>
@@ -7728,7 +7737,7 @@
       <c r="O23" s="25"/>
       <c r="P23" s="25"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C24" s="26" t="s">
         <v>137</v>
       </c>
@@ -7756,7 +7765,7 @@
       <c r="O24" s="25"/>
       <c r="P24" s="25"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C25" s="26" t="s">
         <v>138</v>
       </c>
@@ -7784,7 +7793,7 @@
       <c r="O25" s="25"/>
       <c r="P25" s="25"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C26" s="26" t="s">
         <v>139</v>
       </c>
@@ -7812,12 +7821,12 @@
       <c r="O26" s="25"/>
       <c r="P26" s="25"/>
     </row>
-    <row r="28" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
         <v>130</v>
       </c>
@@ -7851,7 +7860,7 @@
       <c r="O29" s="28"/>
       <c r="P29" s="28"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>41</v>
@@ -7883,7 +7892,7 @@
       <c r="O30" s="25"/>
       <c r="P30" s="25"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C31" s="26" t="s">
         <v>137</v>
       </c>
@@ -7911,7 +7920,7 @@
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C32" s="26" t="s">
         <v>53</v>
       </c>
@@ -7939,7 +7948,7 @@
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C33" s="26" t="s">
         <v>52</v>
       </c>
@@ -7967,7 +7976,7 @@
       <c r="O33" s="25"/>
       <c r="P33" s="25"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>40</v>
       </c>
@@ -7998,7 +8007,7 @@
       <c r="O34" s="25"/>
       <c r="P34" s="25"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C35" s="26" t="s">
         <v>137</v>
       </c>
@@ -8026,7 +8035,7 @@
       <c r="O35" s="25"/>
       <c r="P35" s="25"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C36" s="26" t="s">
         <v>53</v>
       </c>
@@ -8054,7 +8063,7 @@
       <c r="O36" s="25"/>
       <c r="P36" s="25"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C37" s="26" t="s">
         <v>52</v>
       </c>
@@ -8082,7 +8091,7 @@
       <c r="O37" s="25"/>
       <c r="P37" s="25"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>49</v>
       </c>
@@ -8113,7 +8122,7 @@
       <c r="O38" s="25"/>
       <c r="P38" s="25"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C39" s="26" t="s">
         <v>137</v>
       </c>
@@ -8141,7 +8150,7 @@
       <c r="O39" s="25"/>
       <c r="P39" s="25"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C40" s="26" t="s">
         <v>53</v>
       </c>
@@ -8169,7 +8178,7 @@
       <c r="O40" s="25"/>
       <c r="P40" s="25"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C41" s="26" t="s">
         <v>52</v>
       </c>
@@ -8197,7 +8206,7 @@
       <c r="O41" s="25"/>
       <c r="P41" s="25"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>48</v>
       </c>
@@ -8228,7 +8237,7 @@
       <c r="O42" s="25"/>
       <c r="P42" s="25"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C43" s="26" t="s">
         <v>137</v>
       </c>
@@ -8256,7 +8265,7 @@
       <c r="O43" s="25"/>
       <c r="P43" s="25"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C44" s="26" t="s">
         <v>53</v>
       </c>
@@ -8284,7 +8293,7 @@
       <c r="O44" s="25"/>
       <c r="P44" s="25"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C45" s="26" t="s">
         <v>52</v>
       </c>
@@ -8312,7 +8321,7 @@
       <c r="O45" s="25"/>
       <c r="P45" s="25"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>39</v>
       </c>
@@ -8343,7 +8352,7 @@
       <c r="O46" s="25"/>
       <c r="P46" s="25"/>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C47" s="26" t="s">
         <v>137</v>
       </c>
@@ -8371,7 +8380,7 @@
       <c r="O47" s="25"/>
       <c r="P47" s="25"/>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C48" s="26" t="s">
         <v>53</v>
       </c>
@@ -8399,7 +8408,7 @@
       <c r="O48" s="25"/>
       <c r="P48" s="25"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C49" s="26" t="s">
         <v>52</v>
       </c>
@@ -8427,7 +8436,7 @@
       <c r="O49" s="25"/>
       <c r="P49" s="25"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>47</v>
       </c>
@@ -8458,7 +8467,7 @@
       <c r="O50" s="25"/>
       <c r="P50" s="25"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C51" s="26" t="s">
         <v>137</v>
       </c>
@@ -8486,7 +8495,7 @@
       <c r="O51" s="25"/>
       <c r="P51" s="25"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C52" s="26" t="s">
         <v>53</v>
       </c>
@@ -8514,7 +8523,7 @@
       <c r="O52" s="25"/>
       <c r="P52" s="25"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C53" s="26" t="s">
         <v>52</v>
       </c>
@@ -8542,16 +8551,16 @@
       <c r="O53" s="25"/>
       <c r="P53" s="25"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C54" s="26"/>
       <c r="D54" s="26"/>
     </row>
-    <row r="55" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:16" s="27" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
         <v>124</v>
       </c>
@@ -8579,7 +8588,7 @@
       <c r="O56" s="28"/>
       <c r="P56" s="28"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="1" t="s">
         <v>46</v>
@@ -8605,7 +8614,7 @@
       <c r="O57" s="25"/>
       <c r="P57" s="25"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C58" s="26" t="s">
         <v>141</v>
       </c>
@@ -8627,7 +8636,7 @@
       <c r="O58" s="25"/>
       <c r="P58" s="25"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>45</v>
       </c>
@@ -8652,7 +8661,7 @@
       <c r="O59" s="25"/>
       <c r="P59" s="25"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C60" s="26" t="s">
         <v>141</v>
       </c>
@@ -8674,7 +8683,7 @@
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>44</v>
       </c>
@@ -8699,7 +8708,7 @@
       <c r="O61" s="25"/>
       <c r="P61" s="25"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C62" s="26" t="s">
         <v>141</v>
       </c>
@@ -8721,16 +8730,16 @@
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C63" s="26"/>
       <c r="D63" s="26"/>
     </row>
-    <row r="64" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:16" s="27" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A65" s="31" t="s">
         <v>121</v>
       </c>
@@ -8764,7 +8773,7 @@
       <c r="O65" s="28"/>
       <c r="P65" s="28"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="51"/>
       <c r="B66" s="1" t="s">
         <v>7</v>
@@ -8796,7 +8805,7 @@
       <c r="O66" s="25"/>
       <c r="P66" s="25"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C67" s="26" t="s">
         <v>143</v>
       </c>
@@ -8824,7 +8833,7 @@
       <c r="O67" s="25"/>
       <c r="P67" s="25"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C68" s="26" t="s">
         <v>144</v>
       </c>
@@ -8852,7 +8861,7 @@
       <c r="O68" s="25"/>
       <c r="P68" s="25"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C69" s="26" t="s">
         <v>131</v>
       </c>
@@ -8880,7 +8889,7 @@
       <c r="O69" s="25"/>
       <c r="P69" s="25"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
         <v>6</v>
       </c>
@@ -8911,7 +8920,7 @@
       <c r="O70" s="25"/>
       <c r="P70" s="25"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C71" s="26" t="s">
         <v>143</v>
       </c>
@@ -8939,7 +8948,7 @@
       <c r="O71" s="25"/>
       <c r="P71" s="25"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C72" s="26" t="s">
         <v>144</v>
       </c>
@@ -8967,7 +8976,7 @@
       <c r="O72" s="25"/>
       <c r="P72" s="25"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C73" s="26" t="s">
         <v>131</v>
       </c>
@@ -8995,7 +9004,7 @@
       <c r="O73" s="25"/>
       <c r="P73" s="25"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
         <v>5</v>
       </c>
@@ -9026,7 +9035,7 @@
       <c r="O74" s="25"/>
       <c r="P74" s="25"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C75" s="26" t="s">
         <v>143</v>
       </c>
@@ -9054,7 +9063,7 @@
       <c r="O75" s="25"/>
       <c r="P75" s="25"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C76" s="26" t="s">
         <v>144</v>
       </c>
@@ -9082,7 +9091,7 @@
       <c r="O76" s="25"/>
       <c r="P76" s="25"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C77" s="26" t="s">
         <v>131</v>
       </c>
@@ -9110,7 +9119,7 @@
       <c r="O77" s="25"/>
       <c r="P77" s="25"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
         <v>3</v>
       </c>
@@ -9141,7 +9150,7 @@
       <c r="O78" s="25"/>
       <c r="P78" s="25"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C79" s="26" t="s">
         <v>143</v>
       </c>
@@ -9169,7 +9178,7 @@
       <c r="O79" s="25"/>
       <c r="P79" s="25"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C80" s="26" t="s">
         <v>144</v>
       </c>
@@ -9197,7 +9206,7 @@
       <c r="O80" s="25"/>
       <c r="P80" s="25"/>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C81" s="26" t="s">
         <v>131</v>
       </c>
@@ -9225,7 +9234,7 @@
       <c r="O81" s="25"/>
       <c r="P81" s="25"/>
     </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="s">
         <v>41</v>
       </c>
@@ -9256,7 +9265,7 @@
       <c r="O82" s="25"/>
       <c r="P82" s="25"/>
     </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C83" s="26" t="s">
         <v>143</v>
       </c>
@@ -9284,7 +9293,7 @@
       <c r="O83" s="25"/>
       <c r="P83" s="25"/>
     </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C84" s="26" t="s">
         <v>144</v>
       </c>
@@ -9312,7 +9321,7 @@
       <c r="O84" s="25"/>
       <c r="P84" s="25"/>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C85" s="26" t="s">
         <v>131</v>
       </c>
@@ -9340,7 +9349,7 @@
       <c r="O85" s="25"/>
       <c r="P85" s="25"/>
     </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="s">
         <v>40</v>
       </c>
@@ -9371,7 +9380,7 @@
       <c r="O86" s="25"/>
       <c r="P86" s="25"/>
     </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="87" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C87" s="26" t="s">
         <v>143</v>
       </c>
@@ -9399,7 +9408,7 @@
       <c r="O87" s="25"/>
       <c r="P87" s="25"/>
     </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C88" s="26" t="s">
         <v>144</v>
       </c>
@@ -9427,7 +9436,7 @@
       <c r="O88" s="25"/>
       <c r="P88" s="25"/>
     </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="89" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C89" s="26" t="s">
         <v>131</v>
       </c>
@@ -9455,7 +9464,7 @@
       <c r="O89" s="25"/>
       <c r="P89" s="25"/>
     </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="90" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
         <v>49</v>
       </c>
@@ -9486,7 +9495,7 @@
       <c r="O90" s="25"/>
       <c r="P90" s="25"/>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C91" s="26" t="s">
         <v>143</v>
       </c>
@@ -9514,7 +9523,7 @@
       <c r="O91" s="25"/>
       <c r="P91" s="25"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C92" s="26" t="s">
         <v>144</v>
       </c>
@@ -9542,7 +9551,7 @@
       <c r="O92" s="25"/>
       <c r="P92" s="25"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C93" s="26" t="s">
         <v>131</v>
       </c>
@@ -9570,7 +9579,7 @@
       <c r="O93" s="25"/>
       <c r="P93" s="25"/>
     </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="94" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B94" s="1" t="s">
         <v>39</v>
       </c>
@@ -9601,7 +9610,7 @@
       <c r="O94" s="25"/>
       <c r="P94" s="25"/>
     </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="95" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C95" s="26" t="s">
         <v>143</v>
       </c>
@@ -9629,7 +9638,7 @@
       <c r="O95" s="25"/>
       <c r="P95" s="25"/>
     </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="96" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C96" s="26" t="s">
         <v>144</v>
       </c>
@@ -9657,7 +9666,7 @@
       <c r="O96" s="25"/>
       <c r="P96" s="25"/>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C97" s="26" t="s">
         <v>131</v>
       </c>
@@ -9685,7 +9694,7 @@
       <c r="O97" s="25"/>
       <c r="P97" s="25"/>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B98" s="1" t="s">
         <v>129</v>
       </c>
@@ -9716,7 +9725,7 @@
       <c r="O98" s="25"/>
       <c r="P98" s="25"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C99" s="26" t="s">
         <v>143</v>
       </c>
@@ -9744,7 +9753,7 @@
       <c r="O99" s="25"/>
       <c r="P99" s="25"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C100" s="26" t="s">
         <v>144</v>
       </c>
@@ -9772,7 +9781,7 @@
       <c r="O100" s="25"/>
       <c r="P100" s="25"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C101" s="26" t="s">
         <v>131</v>
       </c>
@@ -9800,12 +9809,12 @@
       <c r="O101" s="25"/>
       <c r="P101" s="25"/>
     </row>
-    <row r="103" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:16" s="27" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A104" s="31" t="s">
         <v>41</v>
       </c>
@@ -9839,7 +9848,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="27"/>
       <c r="C105" s="26" t="s">
@@ -9869,7 +9878,7 @@
       <c r="O105" s="25"/>
       <c r="P105" s="25"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C106" s="26" t="s">
         <v>143</v>
       </c>
@@ -9897,7 +9906,7 @@
       <c r="O106" s="25"/>
       <c r="P106" s="25"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C107" s="26" t="s">
         <v>144</v>
       </c>
@@ -9925,7 +9934,7 @@
       <c r="O107" s="25"/>
       <c r="P107" s="25"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C108" s="26" t="s">
         <v>131</v>
       </c>
@@ -9953,7 +9962,7 @@
       <c r="O108" s="25"/>
       <c r="P108" s="25"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
     </row>
   </sheetData>
@@ -9973,24 +9982,24 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
         <v>132</v>
       </c>
@@ -10011,7 +10020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>65</v>
       </c>
@@ -10031,7 +10040,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="6" t="s">
         <v>128</v>
@@ -10052,12 +10061,12 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>62</v>
       </c>
@@ -10077,7 +10086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>61</v>
       </c>
@@ -10097,7 +10106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>89</v>
       </c>
@@ -10117,7 +10126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -10125,12 +10134,12 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="3" t="s">
         <v>152</v>
@@ -10151,16 +10160,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="51" t="s">
         <v>130</v>
       </c>
@@ -10183,7 +10192,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="6" t="s">
         <v>58</v>
@@ -10204,7 +10213,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
         <v>124</v>
       </c>
@@ -10227,13 +10236,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" spans="1:6" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:6" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="43" t="s">
         <v>27</v>
       </c>
@@ -10247,7 +10256,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>118</v>
       </c>
@@ -10282,7 +10291,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47" style="1" customWidth="1"/>
     <col min="2" max="6" width="14.5" style="1"/>
@@ -10291,7 +10300,7 @@
     <col min="9" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>73</v>
       </c>
@@ -10309,7 +10318,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
         <v>72</v>
       </c>
@@ -10329,7 +10338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
       <c r="B3" s="34" t="s">
         <v>67</v>
@@ -10347,7 +10356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
         <v>148</v>
       </c>
@@ -10367,7 +10376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="34"/>
       <c r="B5" s="34" t="s">
         <v>67</v>
@@ -10385,7 +10394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
         <v>158</v>
       </c>
@@ -10405,7 +10414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="34"/>
       <c r="B7" s="34" t="s">
         <v>67</v>
@@ -10423,7 +10432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
         <v>70</v>
       </c>
@@ -10443,7 +10452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34"/>
       <c r="B9" s="34" t="s">
         <v>67</v>
@@ -10461,7 +10470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
         <v>69</v>
       </c>
@@ -10481,7 +10490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34"/>
       <c r="B11" s="34" t="s">
         <v>67</v>
@@ -10499,7 +10508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="34" t="s">
         <v>71</v>
       </c>
@@ -10519,7 +10528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="34"/>
       <c r="B13" s="34" t="s">
         <v>67</v>
@@ -10537,10 +10546,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="34"/>
     </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="34"/>
     </row>
   </sheetData>
@@ -10560,15 +10569,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="15" width="13.5" style="1" customWidth="1"/>
     <col min="16" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="22" t="s">
@@ -10611,12 +10620,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="35" t="s">
         <v>127</v>
       </c>
@@ -10660,7 +10669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="35" t="s">
         <v>149</v>
       </c>
@@ -10704,7 +10713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="35" t="s">
         <v>159</v>
       </c>
@@ -10748,7 +10757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="35" t="s">
         <v>150</v>
       </c>
@@ -10792,7 +10801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="35" t="s">
         <v>151</v>
       </c>
@@ -10836,7 +10845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="34" t="s">
         <v>148</v>
       </c>
@@ -10880,7 +10889,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="34" t="s">
         <v>158</v>
       </c>
@@ -10924,7 +10933,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="35" t="s">
         <v>70</v>
       </c>
@@ -10968,7 +10977,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="34" t="s">
         <v>61</v>
       </c>
@@ -11012,7 +11021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12" s="35" t="s">
         <v>69</v>
       </c>
@@ -11056,7 +11065,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="35" t="s">
         <v>79</v>
       </c>
@@ -11100,7 +11109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="35" t="s">
         <v>71</v>
       </c>
@@ -11144,13 +11153,13 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="35"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="34" t="s">
         <v>75</v>
       </c>
@@ -11194,7 +11203,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="34" t="s">
         <v>74</v>
       </c>
@@ -11238,7 +11247,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="34" t="s">
         <v>76</v>
       </c>
@@ -11282,7 +11291,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="34" t="s">
         <v>77</v>
       </c>
@@ -11326,20 +11335,20 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="26"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="26"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="26"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="26"/>
     </row>
   </sheetData>
-  <sortState ref="B3:O14">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:O14">
     <sortCondition ref="B3:B14"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>